<commit_message>
update system modelling settings
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/output_parameters.xlsx
+++ b/spine_rts-gmlc/datasets/output_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="obj_output" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>report</t>
   </si>
   <si>
-    <t>report_1</t>
-  </si>
-  <si>
     <t>report__output</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>units_available</t>
+  </si>
+  <si>
+    <t>result_temp</t>
   </si>
 </sst>
 </file>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,62 +894,63 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -957,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +985,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1010,7 +1011,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1030,37 +1031,37 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1068,10 +1069,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1079,10 +1080,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1090,24 +1091,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
extend the linear piecewise heat rates to the bus detailed model with considering ptdf
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/output_parameters.xlsx
+++ b/spine_rts-gmlc/datasets/output_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="obj_output" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="31">
   <si>
     <t>rel_class_name</t>
   </si>
@@ -81,6 +81,39 @@
   </si>
   <si>
     <t>total_costs</t>
+  </si>
+  <si>
+    <t>start_up_costs</t>
+  </si>
+  <si>
+    <t>shut_down_costs</t>
+  </si>
+  <si>
+    <t>operating_costs</t>
+  </si>
+  <si>
+    <t>fixed_om_costs</t>
+  </si>
+  <si>
+    <t>variable_om_costs</t>
+  </si>
+  <si>
+    <t>ramp_costs</t>
+  </si>
+  <si>
+    <t>res_proc_costs</t>
+  </si>
+  <si>
+    <t>renewable_curtailment_costs</t>
+  </si>
+  <si>
+    <t>taxes</t>
+  </si>
+  <si>
+    <t>connection_flow_costs</t>
+  </si>
+  <si>
+    <t>investment_costs</t>
   </si>
 </sst>
 </file>
@@ -889,20 +922,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -910,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -918,7 +951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -926,31 +959,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -958,39 +991,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -998,19 +1031,107 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1028,17 +1149,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="34.453125" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1054,16 +1175,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
   </sheetData>
@@ -1076,20 +1197,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1111,7 +1232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1122,29 +1243,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1152,10 +1273,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1166,29 +1287,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1196,10 +1317,10 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1207,10 +1328,10 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1221,7 +1342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1229,81 +1350,169 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update output terms w.r.t. SpineOpt development
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/output_parameters.xlsx
+++ b/spine_rts-gmlc/datasets/output_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="obj_output" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="41">
   <si>
     <t>rel_class_name</t>
   </si>
@@ -62,9 +62,6 @@
     <t>units_available</t>
   </si>
   <si>
-    <t>result_temp</t>
-  </si>
-  <si>
     <t>node_injection</t>
   </si>
   <si>
@@ -117,6 +114,36 @@
   </si>
   <si>
     <t>res_start_up_costs</t>
+  </si>
+  <si>
+    <t>units_mothballed</t>
+  </si>
+  <si>
+    <t>unit_flow_op</t>
+  </si>
+  <si>
+    <t>units_invested</t>
+  </si>
+  <si>
+    <t>nonspin_ramp_up_unit_flow</t>
+  </si>
+  <si>
+    <t>start_up_unit_flow</t>
+  </si>
+  <si>
+    <t>units_invested_available</t>
+  </si>
+  <si>
+    <t>ramp_up_unit_flow</t>
+  </si>
+  <si>
+    <t>nonspin_units_starting_up</t>
+  </si>
+  <si>
+    <t>result_objective_terms</t>
+  </si>
+  <si>
+    <t>result_variables</t>
   </si>
 </sst>
 </file>
@@ -934,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="B34" sqref="B2:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1016,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1024,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1032,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1040,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1048,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1056,7 +1083,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1064,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1072,7 +1099,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1080,7 +1107,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1088,7 +1115,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1096,7 +1123,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1104,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1112,7 +1139,7 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1120,7 +1147,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1128,7 +1155,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1136,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1144,7 +1171,79 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1257,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1184,11 +1283,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="1"/>
@@ -1209,14 +1313,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
@@ -1238,7 +1342,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1249,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1260,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -1271,7 +1375,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1282,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1293,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1304,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1315,10 +1419,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1326,10 +1430,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1337,10 +1441,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1348,10 +1452,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1359,10 +1463,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1371,10 +1475,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1383,10 +1487,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1395,10 +1499,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -1407,10 +1511,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -1419,10 +1523,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -1431,10 +1535,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -1443,10 +1547,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -1455,10 +1559,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -1467,10 +1571,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1479,10 +1583,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1491,10 +1595,10 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -1503,10 +1607,10 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -1515,38 +1619,102 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="B27" s="1"/>
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="2"/>
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="B29" s="2"/>
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="2"/>
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" s="2"/>
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="B35" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renewal of data w.r.t. current updates
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/output_parameters.xlsx
+++ b/spine_rts-gmlc/datasets/output_parameters.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="39">
   <si>
     <t>rel_class_name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>ramp_costs</t>
   </si>
   <si>
-    <t>res_proc_costs</t>
-  </si>
-  <si>
     <t>renewable_curtailment_costs</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>investment_costs</t>
   </si>
   <si>
-    <t>res_start_up_costs</t>
-  </si>
-  <si>
     <t>units_mothballed</t>
   </si>
   <si>
@@ -137,13 +131,13 @@
     <t>ramp_up_unit_flow</t>
   </si>
   <si>
-    <t>nonspin_units_starting_up</t>
-  </si>
-  <si>
     <t>all_objective_terms</t>
   </si>
   <si>
     <t>all_variables</t>
+  </si>
+  <si>
+    <t>nonspin_units_started_up</t>
   </si>
 </sst>
 </file>
@@ -961,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B34"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1067,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1075,7 +1069,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1083,7 +1077,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1091,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1099,7 +1093,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1107,7 +1101,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1115,7 +1109,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1155,7 +1149,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1179,7 +1173,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1211,7 +1205,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1219,7 +1213,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1227,23 +1221,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1235,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1283,7 +1261,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1291,7 +1269,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1311,17 +1289,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -1342,7 +1320,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1353,7 +1331,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1364,7 +1342,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -1375,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1386,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1397,7 +1375,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1408,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1419,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1430,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -1441,7 +1419,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -1452,10 +1430,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1463,10 +1441,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1475,10 +1453,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1487,10 +1465,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1499,10 +1477,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -1511,10 +1489,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -1523,10 +1501,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -1535,7 +1513,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1547,7 +1525,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -1559,7 +1537,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -1571,7 +1549,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -1583,10 +1561,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1595,7 +1573,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -1607,7 +1585,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1619,10 +1597,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3"/>
     </row>
@@ -1631,7 +1609,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
@@ -1642,7 +1620,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
@@ -1653,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1664,10 +1642,10 @@
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1675,10 +1653,10 @@
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1686,36 +1664,11 @@
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>